<commit_message>
general alarm time update
</commit_message>
<xml_diff>
--- a/01_Logger/02_Modular_Logger/03_Software/media/LED_signals_rev1_1.xlsx
+++ b/01_Logger/02_Modular_Logger/03_Software/media/LED_signals_rev1_1.xlsx
@@ -680,7 +680,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -801,7 +801,7 @@
         <v>0.1</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>17</v>

</xml_diff>